<commit_message>
1) Fix misspelling on QB description 2) remove Date Column from PostBundle 3) Added login form to both PostBundle and ScanUploader
</commit_message>
<xml_diff>
--- a/PostBundle/PostBundle/PostBundle.xlsx
+++ b/PostBundle/PostBundle/PostBundle.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8010" yWindow="2760" windowWidth="16710" windowHeight="7110"/>
+    <workbookView xWindow="-3930" yWindow="3390" windowWidth="13905" windowHeight="7290"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,9 +16,9 @@
     <definedName name="BundleFund">Sheet1!$B$4</definedName>
     <definedName name="BundleId">Sheet1!$B$1</definedName>
     <definedName name="BundleTotal">Sheet1!$B$2</definedName>
-    <definedName name="Date">Sheet1!$C$8:$C$9</definedName>
-    <definedName name="Fund">Sheet1!$D$8:$D$9</definedName>
-    <definedName name="Name">Sheet1!$E$8:$E$9</definedName>
+    <definedName name="Date">Sheet1!#REF!</definedName>
+    <definedName name="Fund">Sheet1!$C$8:$C$9</definedName>
+    <definedName name="Name">Sheet1!$D$8:$D$9</definedName>
     <definedName name="PeopleId">Sheet1!$A$8:$A$9</definedName>
     <definedName name="Pledge">Sheet1!$B$5</definedName>
   </definedNames>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>BundleId</t>
   </si>
@@ -182,7 +182,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -210,10 +210,6 @@
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -236,9 +232,15 @@
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+  <dxfs count="16">
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -253,35 +255,23 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
@@ -359,22 +349,21 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="3">
-      <tableStyleElement type="wholeTable" dxfId="17"/>
-      <tableStyleElement type="headerRow" dxfId="16"/>
-      <tableStyleElement type="totalRow" dxfId="15"/>
+      <tableStyleElement type="wholeTable" dxfId="15"/>
+      <tableStyleElement type="headerRow" dxfId="14"/>
+      <tableStyleElement type="totalRow" dxfId="13"/>
     </tableStyle>
   </tableStyles>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A7:E9" totalsRowCount="1" headerRowDxfId="14" dataCellStyle="Normal" totalsRowCellStyle="Normal">
-  <tableColumns count="5">
-    <tableColumn id="1" name="PeopleId" totalsRowLabel="Total" dataDxfId="13" totalsRowDxfId="6" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Amount" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="5" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Date" dataDxfId="11" totalsRowDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Fund" dataDxfId="1" totalsRowDxfId="3" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Name" dataDxfId="0" totalsRowDxfId="2" dataCellStyle="Normal"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A7:D9" totalsRowCount="1" headerRowDxfId="12" dataCellStyle="Normal" totalsRowCellStyle="Normal">
+  <tableColumns count="4">
+    <tableColumn id="1" name="PeopleId" totalsRowLabel="Total" dataDxfId="11" totalsRowDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Amount" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Fund" dataDxfId="7" totalsRowDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Name" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -383,8 +372,8 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:B3" totalsRowCount="1">
   <tableColumns count="2">
-    <tableColumn id="1" name="Fund" totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="2" name="Total" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="7">
+    <tableColumn id="1" name="Fund" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="2" name="Total" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0">
       <calculatedColumnFormula>SUMIF(Table1[Fund],[Fund],Table1[Amount])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -678,83 +667,78 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:12">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:12">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6"/>
-      <c r="M2">
+      <c r="L2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:12">
       <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="M3">
+      <c r="L3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:12">
+      <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="5"/>
     </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:12">
+      <c r="A5" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="D7" s="17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="17"/>
+    <row r="8" spans="1:12">
+      <c r="A8" s="15"/>
       <c r="B8" s="11"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="20"/>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="C8" s="8"/>
+      <c r="D8" s="18"/>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -762,15 +746,14 @@
         <f>SUBTOTAL(109,[Amount])</f>
         <v>0</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="18"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="16"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>$M$2:$M$3</formula1>
+      <formula1>$L$2:$L$3</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>